<commit_message>
- conformed VMA_MaxHostStereo send/recieve objects to append .VMA as in other patches - renamed
</commit_message>
<xml_diff>
--- a/DevFiles/SamplesDevDatabase.xlsx
+++ b/DevFiles/SamplesDevDatabase.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-24780" yWindow="4360" windowWidth="24300" windowHeight="23920" tabRatio="500"/>
+    <workbookView xWindow="-24780" yWindow="4360" windowWidth="24180" windowHeight="23920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="102">
   <si>
     <t>arcade</t>
   </si>
@@ -293,13 +293,46 @@
   </si>
   <si>
     <t>bookmarked</t>
+  </si>
+  <si>
+    <t>abandoned this theme</t>
+  </si>
+  <si>
+    <t>through 20/47 pages</t>
+  </si>
+  <si>
+    <t>not useful</t>
+  </si>
+  <si>
+    <t>not different from Laser</t>
+  </si>
+  <si>
+    <t>too general (2687 sounds)</t>
+  </si>
+  <si>
+    <t>too general</t>
+  </si>
+  <si>
+    <t>a couple in atari</t>
+  </si>
+  <si>
+    <t>bookmarked from20/51pgs</t>
+  </si>
+  <si>
+    <t>bookmarked 20/45pages</t>
+  </si>
+  <si>
+    <t>fight</t>
+  </si>
+  <si>
+    <t>ChucklesGiggles bookmark downloaded</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -338,13 +371,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -367,11 +411,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -755,7 +802,7 @@
   <dimension ref="A1:I97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -781,11 +828,17 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B3" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B4" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
@@ -823,6 +876,9 @@
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B10" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
@@ -836,11 +892,17 @@
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B13" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="5" t="s">
         <v>9</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -852,11 +914,17 @@
       <c r="A16" s="1" t="s">
         <v>79</v>
       </c>
+      <c r="B16" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
         <v>80</v>
       </c>
+      <c r="B17" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
@@ -929,150 +997,180 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:2">
       <c r="A34" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:2">
       <c r="A35" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:2">
       <c r="A36" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:2">
       <c r="A37" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:2">
       <c r="A38" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="39" spans="1:1">
+      <c r="B38" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
       <c r="A39" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="40" spans="1:1">
+      <c r="B39" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
       <c r="A40" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:2">
       <c r="A41" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:2">
       <c r="A42" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:2">
       <c r="A43" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:2">
       <c r="A45" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:2">
       <c r="A46" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:2">
       <c r="A47" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:2">
       <c r="A48" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:2">
       <c r="A49" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:2">
       <c r="A50" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:2">
       <c r="A51" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:2">
       <c r="A52" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:2">
       <c r="A53" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:2">
       <c r="A55" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="56" spans="1:1">
+      <c r="B55" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
       <c r="A56" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="57" spans="1:1">
+      <c r="B56" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
       <c r="A57" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="58" spans="1:1">
+      <c r="B57" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
       <c r="A58" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="59" spans="1:1">
+      <c r="B58" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
       <c r="A59" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="60" spans="1:1">
+      <c r="B59" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
       <c r="A60" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="61" spans="1:1">
+      <c r="B60" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
       <c r="A61" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="62" spans="1:1">
+      <c r="B61" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
       <c r="A62" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="63" spans="1:1">
+      <c r="B62" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
       <c r="A63" s="1"/>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:2">
       <c r="A64" s="1" t="s">
         <v>56</v>
       </c>
@@ -1096,6 +1194,9 @@
       <c r="A69" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="B69" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="70" spans="1:8">
       <c r="A70" s="1" t="s">
@@ -1118,6 +1219,14 @@
       </c>
       <c r="H73" s="1"/>
     </row>
+    <row r="74" spans="1:8">
+      <c r="A74" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B74" t="s">
+        <v>90</v>
+      </c>
+    </row>
     <row r="75" spans="1:8">
       <c r="A75" s="1" t="s">
         <v>77</v>
@@ -1142,7 +1251,12 @@
       <c r="A79" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B79" s="1"/>
+      <c r="B79" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C79" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="80" spans="1:8">
       <c r="A80" s="1" t="s">
@@ -1267,52 +1381,48 @@
     <hyperlink ref="A51" r:id="rId39"/>
     <hyperlink ref="A52" r:id="rId40"/>
     <hyperlink ref="A53" r:id="rId41"/>
-    <hyperlink ref="A55" r:id="rId42"/>
-    <hyperlink ref="A56" r:id="rId43"/>
-    <hyperlink ref="A57" r:id="rId44"/>
-    <hyperlink ref="A58" r:id="rId45"/>
-    <hyperlink ref="A59" r:id="rId46"/>
-    <hyperlink ref="A60" r:id="rId47"/>
-    <hyperlink ref="A61" r:id="rId48"/>
-    <hyperlink ref="A65" r:id="rId49"/>
-    <hyperlink ref="A66" r:id="rId50"/>
-    <hyperlink ref="A62" r:id="rId51"/>
-    <hyperlink ref="A67" r:id="rId52"/>
-    <hyperlink ref="A73" r:id="rId53"/>
-    <hyperlink ref="A69" r:id="rId54"/>
-    <hyperlink ref="A70" r:id="rId55"/>
-    <hyperlink ref="A71" r:id="rId56"/>
-    <hyperlink ref="A72" r:id="rId57"/>
-    <hyperlink ref="A64" r:id="rId58"/>
-    <hyperlink ref="A78" r:id="rId59"/>
-    <hyperlink ref="A76" r:id="rId60"/>
-    <hyperlink ref="A81" r:id="rId61"/>
-    <hyperlink ref="A80" r:id="rId62"/>
-    <hyperlink ref="A83" r:id="rId63"/>
-    <hyperlink ref="A84" r:id="rId64"/>
-    <hyperlink ref="A82" r:id="rId65"/>
-    <hyperlink ref="A75" r:id="rId66"/>
-    <hyperlink ref="A79" r:id="rId67"/>
-    <hyperlink ref="A86" r:id="rId68"/>
-    <hyperlink ref="A87" r:id="rId69"/>
-    <hyperlink ref="A88" r:id="rId70"/>
-    <hyperlink ref="A89" r:id="rId71"/>
-    <hyperlink ref="A90" r:id="rId72"/>
-    <hyperlink ref="A77" r:id="rId73"/>
-    <hyperlink ref="A94" r:id="rId74"/>
-    <hyperlink ref="A93" r:id="rId75"/>
-    <hyperlink ref="A92" r:id="rId76"/>
-    <hyperlink ref="A95" r:id="rId77"/>
-    <hyperlink ref="A96" r:id="rId78"/>
-    <hyperlink ref="A97" r:id="rId79"/>
-    <hyperlink ref="A34" r:id="rId80"/>
-    <hyperlink ref="A33" r:id="rId81"/>
-    <hyperlink ref="A15" r:id="rId82"/>
-    <hyperlink ref="A16" r:id="rId83"/>
-    <hyperlink ref="A17" r:id="rId84"/>
-    <hyperlink ref="C7" r:id="rId85"/>
-    <hyperlink ref="A9" r:id="rId86"/>
-    <hyperlink ref="C30" r:id="rId87"/>
+    <hyperlink ref="A56" r:id="rId42"/>
+    <hyperlink ref="A57" r:id="rId43"/>
+    <hyperlink ref="A58" r:id="rId44"/>
+    <hyperlink ref="A73" r:id="rId45"/>
+    <hyperlink ref="A60" r:id="rId46"/>
+    <hyperlink ref="A61" r:id="rId47"/>
+    <hyperlink ref="A62" r:id="rId48"/>
+    <hyperlink ref="A72" r:id="rId49"/>
+    <hyperlink ref="A55" r:id="rId50"/>
+    <hyperlink ref="A78" r:id="rId51"/>
+    <hyperlink ref="A76" r:id="rId52"/>
+    <hyperlink ref="A81" r:id="rId53"/>
+    <hyperlink ref="A80" r:id="rId54"/>
+    <hyperlink ref="A83" r:id="rId55"/>
+    <hyperlink ref="A84" r:id="rId56"/>
+    <hyperlink ref="A82" r:id="rId57"/>
+    <hyperlink ref="A75" r:id="rId58"/>
+    <hyperlink ref="A79" r:id="rId59"/>
+    <hyperlink ref="A86" r:id="rId60"/>
+    <hyperlink ref="A87" r:id="rId61"/>
+    <hyperlink ref="A88" r:id="rId62"/>
+    <hyperlink ref="A89" r:id="rId63"/>
+    <hyperlink ref="A90" r:id="rId64"/>
+    <hyperlink ref="A77" r:id="rId65"/>
+    <hyperlink ref="A94" r:id="rId66"/>
+    <hyperlink ref="A93" r:id="rId67"/>
+    <hyperlink ref="A92" r:id="rId68"/>
+    <hyperlink ref="A95" r:id="rId69"/>
+    <hyperlink ref="A96" r:id="rId70"/>
+    <hyperlink ref="A97" r:id="rId71"/>
+    <hyperlink ref="A34" r:id="rId72"/>
+    <hyperlink ref="A33" r:id="rId73"/>
+    <hyperlink ref="A15" r:id="rId74"/>
+    <hyperlink ref="A16" r:id="rId75"/>
+    <hyperlink ref="A17" r:id="rId76"/>
+    <hyperlink ref="C7" r:id="rId77"/>
+    <hyperlink ref="A9" r:id="rId78"/>
+    <hyperlink ref="C30" r:id="rId79"/>
+    <hyperlink ref="A59" r:id="rId80"/>
+    <hyperlink ref="A69" r:id="rId81"/>
+    <hyperlink ref="A70" r:id="rId82"/>
+    <hyperlink ref="A74" r:id="rId83" location="sound"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>